<commit_message>
working in the viewer sidebar
</commit_message>
<xml_diff>
--- a/database/Libro1.xlsx
+++ b/database/Libro1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16920" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16920" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Family" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="63">
   <si>
     <t>name</t>
   </si>
@@ -209,6 +209,12 @@
   </si>
   <si>
     <t>true</t>
+  </si>
+  <si>
+    <t>upf_00205</t>
+  </si>
+  <si>
+    <t>FJSL young brother</t>
   </si>
 </sst>
 </file>
@@ -526,7 +532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -586,10 +592,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -700,9 +706,6 @@
       <c r="C5" t="s">
         <v>43</v>
       </c>
-      <c r="D5" t="s">
-        <v>44</v>
-      </c>
       <c r="F5" t="s">
         <v>26</v>
       </c>
@@ -715,10 +718,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
         <v>42</v>
@@ -738,19 +741,19 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
         <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G7" t="s">
         <v>5</v>
@@ -761,19 +764,22 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
         <v>42</v>
       </c>
-      <c r="F8" t="s">
-        <v>29</v>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
       </c>
       <c r="G8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H8" t="s">
         <v>46</v>
@@ -781,16 +787,16 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" t="s">
         <v>29</v>
-      </c>
-      <c r="B9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" t="s">
-        <v>30</v>
       </c>
       <c r="G9" t="s">
         <v>7</v>
@@ -801,19 +807,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
         <v>43</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>30</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
       </c>
       <c r="G10" t="s">
         <v>7</v>
@@ -824,10 +827,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
         <v>43</v>
@@ -842,6 +845,29 @@
         <v>7</v>
       </c>
       <c r="H11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" t="s">
         <v>46</v>
       </c>
     </row>
@@ -852,10 +878,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -969,10 +995,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="C6" s="1">
-        <v>24473</v>
+        <v>28856</v>
       </c>
       <c r="E6" t="s">
         <v>47</v>
@@ -986,26 +1012,29 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>28</v>
+      </c>
+      <c r="C7" s="1">
+        <v>24473</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" t="s">
-        <v>48</v>
-      </c>
-      <c r="I8" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
         <v>47</v>
@@ -1019,51 +1048,36 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10">
-        <v>446093</v>
-      </c>
-      <c r="C10" s="1">
-        <v>34335</v>
-      </c>
-      <c r="D10" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G10" t="s">
-        <v>51</v>
-      </c>
-      <c r="H10" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="I10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11">
-        <v>490754</v>
+        <v>446093</v>
       </c>
       <c r="C11" s="1">
-        <v>35796</v>
+        <v>34335</v>
       </c>
       <c r="D11" t="s">
         <v>54</v>
       </c>
       <c r="E11" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G11" t="s">
         <v>51</v>
@@ -1072,6 +1086,35 @@
         <v>52</v>
       </c>
       <c r="I11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12">
+        <v>490754</v>
+      </c>
+      <c r="C12" s="1">
+        <v>35796</v>
+      </c>
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>